<commit_message>
Typo corrected in RatcliffeObesrhelp
</commit_message>
<xml_diff>
--- a/toolbox/datasets/multivariate_regression/continents-according-to-our-world-in-data.xlsx
+++ b/toolbox/datasets/multivariate_regression/continents-according-to-our-world-in-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA\toolbox\utilities\privateFS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MATLAB\FSDAgit\FSDA\toolbox\datasets\multivariate_regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805C9D7C-7C3B-44E8-BD61-8922EB326E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF20F9A2-4B34-4783-8351-97197F19B7AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="2" xr2:uid="{0F1F91C3-AB88-4B1C-B272-861E8199DE24}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{0F1F91C3-AB88-4B1C-B272-861E8199DE24}"/>
   </bookViews>
   <sheets>
     <sheet name="CountryContinent" sheetId="1" r:id="rId1"/>
@@ -4235,7 +4235,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4421,12 +4421,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -4588,7 +4582,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4603,7 +4597,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4995,8 +4988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{801C42A8-5B9E-4875-A425-B285D25643D0}">
   <dimension ref="A1:E286"/>
   <sheetViews>
-    <sheetView topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="A252" sqref="A252"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -6108,7 +6101,7 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="6" t="s">
+      <c r="A59" t="s">
         <v>123</v>
       </c>
       <c r="B59" t="s">
@@ -6298,7 +6291,7 @@
       </c>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="6" t="s">
+      <c r="A69" t="s">
         <v>143</v>
       </c>
       <c r="B69" t="s">
@@ -15730,7 +15723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17363E50-6B9F-4AD4-8E80-4D0DCC74AF60}">
   <dimension ref="A1:B225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
+    <sheetView topLeftCell="A190" workbookViewId="0">
       <selection activeCell="B210" sqref="B210"/>
     </sheetView>
   </sheetViews>

</xml_diff>